<commit_message>
2022 Agustus 08 Senin
</commit_message>
<xml_diff>
--- a/Data Files/Data/Kino.xlsx
+++ b/Data Files/Data/Kino.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Powercommerce\Katalon Studio\Kino\Data Files\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42F4ABA-4E5A-483B-AD8E-605ECD1F93E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81BDA26-81DB-48C5-A804-2ACE851F0FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" activeTab="5" xr2:uid="{8EEA7C8B-4B21-4770-8264-34E3959B9269}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{8EEA7C8B-4B21-4770-8264-34E3959B9269}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="1" r:id="rId1"/>
     <sheet name="SignIn" sheetId="3" r:id="rId2"/>
     <sheet name="ForgetPass" sheetId="4" r:id="rId3"/>
     <sheet name="Temp" sheetId="5" r:id="rId4"/>
-    <sheet name="Contoh" sheetId="6" r:id="rId5"/>
+    <sheet name="Transaction" sheetId="6" r:id="rId5"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="78">
   <si>
     <t>password</t>
   </si>
@@ -213,13 +213,73 @@
   </si>
   <si>
     <t>fotoToko</t>
+  </si>
+  <si>
+    <t>checkProduct</t>
+  </si>
+  <si>
+    <t>typePaymentMethod</t>
+  </si>
+  <si>
+    <t>namePayment</t>
+  </si>
+  <si>
+    <t>useKinoKoin</t>
+  </si>
+  <si>
+    <t>typeKinoKoin</t>
+  </si>
+  <si>
+    <t>kinoKoin</t>
+  </si>
+  <si>
+    <t>va</t>
+  </si>
+  <si>
+    <t>mandiri</t>
+  </si>
+  <si>
+    <t>bt</t>
+  </si>
+  <si>
+    <t>tidak</t>
+  </si>
+  <si>
+    <t>Segar Sari c jeruk, 4, ctn</t>
+  </si>
+  <si>
+    <t>ya</t>
+  </si>
+  <si>
+    <t>semua</t>
+  </si>
+  <si>
+    <t>sebagian</t>
+  </si>
+  <si>
+    <t>potensialSebelum</t>
+  </si>
+  <si>
+    <t>potensialSesudah</t>
+  </si>
+  <si>
+    <t>totalKinoKoin</t>
+  </si>
+  <si>
+    <t>kinoKoinSetelahTerpotong</t>
+  </si>
+  <si>
+    <t>totalTagihan</t>
+  </si>
+  <si>
+    <t>cap panda can, 4, ctn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +298,12 @@
     <font>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -264,12 +330,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1137,39 +1205,169 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E88151D-C7BC-4828-A435-2594E6EDABCA}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{1F82F5A1-5D7D-4A34-8865-BBCD03BBFAE8}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1177,7 +1375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE3BB0A-CF0E-4D2C-8281-475FBED3503A}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>